<commit_message>
Deploying to gh-pages from  @ c72c71cf38c394b5cc51b6e6fb312176b91f6a1d 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.4.2.1.xlsx
+++ b/en/downloads/data-excel/16.4.2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>16.4.2.1 Количество изъятого и добровольно сданного огнестрельного оружия</t>
   </si>
@@ -50,13 +50,25 @@
   </si>
   <si>
     <t>Алынган ок атуучу куралдар</t>
+  </si>
+  <si>
+    <t>(единиц)</t>
+  </si>
+  <si>
+    <t>(бирдик)</t>
+  </si>
+  <si>
+    <t>(units)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +98,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -148,6 +167,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,20 +484,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="35.28515625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="35.85546875" style="1" customWidth="1"/>
     <col min="4" max="7" width="9.7109375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -477,106 +506,137 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+    <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="4">
         <v>2016</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E4" s="4">
         <v>2017</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F4" s="4">
         <v>2018</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G4" s="4">
         <v>2019</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H4" s="4">
         <v>2020</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I4" s="4">
         <v>2021</v>
       </c>
+      <c r="J4" s="4">
+        <v>2022</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="5" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <v>153</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E5" s="6">
         <v>196</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F5" s="6">
         <v>232</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G5" s="1">
         <v>146</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H5" s="1">
         <v>158</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I5" s="1">
         <v>149</v>
       </c>
+      <c r="J5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="1">
+        <v>219</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" s="5">
         <v>217</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E6" s="5">
         <v>399</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F6" s="5">
         <v>296</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G6" s="5">
         <v>127</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H6" s="5">
         <v>397</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I6" s="5">
         <v>159</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="5">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>